<commit_message>
+ added menu: guidelines choice (multi select)  => now it is possible to crop w/o any guideline or w/ all of them + updated translations (new strings, one ID change) ~ TAB -> 4xSPC convert
</commit_message>
<xml_diff>
--- a/translations/code/translations.xlsx
+++ b/translations/code/translations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="111">
   <si>
     <t>AvailLangs</t>
   </si>
@@ -58,9 +58,6 @@
     <t>Stwórz maskę kadrującą</t>
   </si>
   <si>
-    <t>cancelCrop</t>
-  </si>
-  <si>
     <t>Cancel</t>
   </si>
   <si>
@@ -233,6 +230,123 @@
   </si>
   <si>
     <t>Wróć do kadrowania</t>
+  </si>
+  <si>
+    <t>chCompMethod</t>
+  </si>
+  <si>
+    <t>Composition method</t>
+  </si>
+  <si>
+    <t>Metoda kompozycji</t>
+  </si>
+  <si>
+    <t>chCompMethodQ</t>
+  </si>
+  <si>
+    <t>Choose composition guidelines</t>
+  </si>
+  <si>
+    <t>Wybierz metodę kompozycji</t>
+  </si>
+  <si>
+    <t>goldenRule</t>
+  </si>
+  <si>
+    <t>Golden Rule</t>
+  </si>
+  <si>
+    <t>Złoty podział</t>
+  </si>
+  <si>
+    <t>ruleOfThirds</t>
+  </si>
+  <si>
+    <t>Rule of Thirds</t>
+  </si>
+  <si>
+    <t>Reguła trzech</t>
+  </si>
+  <si>
+    <t>goldenSpiralBL</t>
+  </si>
+  <si>
+    <t>Golden Spiral bottom-left</t>
+  </si>
+  <si>
+    <t>Złota spirala lewo-dół</t>
+  </si>
+  <si>
+    <t>goldenSpiralTL</t>
+  </si>
+  <si>
+    <t>Golden Spiral top-left</t>
+  </si>
+  <si>
+    <t>Złota spirala lewo-góra</t>
+  </si>
+  <si>
+    <t>goldenSpiralTR</t>
+  </si>
+  <si>
+    <t>Golden Spiral top-right</t>
+  </si>
+  <si>
+    <t>Złota spirala prawo-góra</t>
+  </si>
+  <si>
+    <t>goldenSpiralBR</t>
+  </si>
+  <si>
+    <t>Golden Spiral bottom-right</t>
+  </si>
+  <si>
+    <t>Złota spirala prawo-dół</t>
+  </si>
+  <si>
+    <t>selectAll</t>
+  </si>
+  <si>
+    <t>Select All</t>
+  </si>
+  <si>
+    <t>Zaznacz wszystkie</t>
+  </si>
+  <si>
+    <t>deselectAll</t>
+  </si>
+  <si>
+    <t>Deselect All</t>
+  </si>
+  <si>
+    <t>Odznacz wszystkie</t>
+  </si>
+  <si>
+    <t>ok</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>cancel</t>
+  </si>
+  <si>
+    <t>All Golden Spirals</t>
+  </si>
+  <si>
+    <t>Wszystkie Złote Spirale</t>
+  </si>
+  <si>
+    <t>Basic rules</t>
+  </si>
+  <si>
+    <t>Podstawowe podziały</t>
+  </si>
+  <si>
+    <t>allGoldenSpirals</t>
+  </si>
+  <si>
+    <t>basicRules</t>
   </si>
 </sst>
 </file>
@@ -626,10 +740,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
@@ -700,222 +814,365 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
+        <v>104</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>18</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
         <v>20</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
         <v>23</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
         <v>29</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>30</v>
-      </c>
-      <c r="C11" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
         <v>35</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>36</v>
-      </c>
-      <c r="C13" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
         <v>38</v>
       </c>
-      <c r="B14" t="s">
-        <v>39</v>
-      </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
         <v>40</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>41</v>
-      </c>
-      <c r="C15" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
         <v>43</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>44</v>
-      </c>
-      <c r="C16" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:3">
       <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
         <v>46</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>47</v>
-      </c>
-      <c r="C17" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" t="s">
         <v>49</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>50</v>
-      </c>
-      <c r="C18" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" t="s">
         <v>52</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>53</v>
-      </c>
-      <c r="C19" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:3">
       <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" t="s">
         <v>55</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>56</v>
-      </c>
-      <c r="C20" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:3">
       <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
         <v>58</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>59</v>
-      </c>
-      <c r="C21" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:3">
       <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
         <v>61</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>62</v>
-      </c>
-      <c r="C22" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:3">
       <c r="A23" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" t="s">
         <v>64</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>65</v>
-      </c>
-      <c r="C23" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:3">
       <c r="A24" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" t="s">
         <v>67</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>68</v>
-      </c>
-      <c r="C24" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" t="s">
+        <v>69</v>
+      </c>
+      <c r="B25" t="s">
         <v>70</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>71</v>
       </c>
-      <c r="C25" t="s">
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
         <v>72</v>
+      </c>
+      <c r="B26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>78</v>
+      </c>
+      <c r="B28" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>81</v>
+      </c>
+      <c r="B29" t="s">
+        <v>82</v>
+      </c>
+      <c r="C29" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>87</v>
+      </c>
+      <c r="B31" t="s">
+        <v>88</v>
+      </c>
+      <c r="C31" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>93</v>
+      </c>
+      <c r="B33" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" t="s">
+        <v>97</v>
+      </c>
+      <c r="C34" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>102</v>
+      </c>
+      <c r="B36" t="s">
+        <v>103</v>
+      </c>
+      <c r="C36" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" t="s">
+        <v>105</v>
+      </c>
+      <c r="C37" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>110</v>
+      </c>
+      <c r="B38" t="s">
+        <v>107</v>
+      </c>
+      <c r="C38" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
German Translation [DE] (script) thanks to Arkadius!
</commit_message>
<xml_diff>
--- a/translations/code/translations.xlsx
+++ b/translations/code/translations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="141">
   <si>
     <t>AvailLangs</t>
   </si>
@@ -25,9 +25,6 @@
     <t>pl</t>
   </si>
   <si>
-    <t>ru</t>
-  </si>
-  <si>
     <t>chCropMethod</t>
   </si>
   <si>
@@ -82,15 +79,6 @@
     <t>Wypełnienie tła</t>
   </si>
   <si>
-    <t>doOutsCrop</t>
-  </si>
-  <si>
-    <t>Do outside cropping (YES) or crop without extending canvas (NO)?</t>
-  </si>
-  <si>
-    <t>Rozszerzyć półtno (TAK) czy przyciąć bez rozszerzania (NIE)?</t>
-  </si>
-  <si>
     <t>-grid</t>
   </si>
   <si>
@@ -347,6 +335,108 @@
   </si>
   <si>
     <t>basicRules</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>Wähle Schnittstil</t>
+  </si>
+  <si>
+    <t>Arbeitsfläche aufteilen</t>
+  </si>
+  <si>
+    <t>Erstelle Schnittmaske</t>
+  </si>
+  <si>
+    <t>Abbrechen</t>
+  </si>
+  <si>
+    <t>Hintergrund auf Ebene</t>
+  </si>
+  <si>
+    <t>Hintergrund füllen</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Rastern</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Skalieren</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Einblenden</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Beschneiden</t>
+  </si>
+  <si>
+    <t>Schnittmaske</t>
+  </si>
+  <si>
+    <t>Trennungsregeln</t>
+  </si>
+  <si>
+    <t>Linien auf %1%%</t>
+  </si>
+  <si>
+    <t>Goldene Diagonale aufwärts</t>
+  </si>
+  <si>
+    <t>Goldene Diagonale abwärts</t>
+  </si>
+  <si>
+    <t>Öffne das Dokument, in dem das Script ablaufen soll.</t>
+  </si>
+  <si>
+    <t>Erweiterung der Arbeitsfläche zeigen</t>
+  </si>
+  <si>
+    <t>Was mache ich mit der Arbeitsfläche?</t>
+  </si>
+  <si>
+    <t>Erweiterte Arbeitsfläche</t>
+  </si>
+  <si>
+    <t>Schnitt ohne Erweiterung</t>
+  </si>
+  <si>
+    <t>Zurück zum Schneiden</t>
+  </si>
+  <si>
+    <t>Kompositionsmethode</t>
+  </si>
+  <si>
+    <t>Auswahl der Kompositionslinien</t>
+  </si>
+  <si>
+    <t>Goldene Regel</t>
+  </si>
+  <si>
+    <t>Drittel-Regel</t>
+  </si>
+  <si>
+    <t>Goldene Spirale unten links</t>
+  </si>
+  <si>
+    <t>Goldene Spirale oben links</t>
+  </si>
+  <si>
+    <t>Goldene Spirale oben rechts</t>
+  </si>
+  <si>
+    <t>Goldene Spirale unten rechts</t>
+  </si>
+  <si>
+    <t>Alles Auswählen</t>
+  </si>
+  <si>
+    <t>Nichts Auswählen</t>
+  </si>
+  <si>
+    <t>Alle Goldenen Spiralen</t>
+  </si>
+  <si>
+    <t>Grundregeln</t>
   </si>
 </sst>
 </file>
@@ -740,18 +830,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:C38"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="15.140625" customWidth="1"/>
     <col min="2" max="2" width="56.140625" customWidth="1"/>
     <col min="3" max="3" width="53.42578125" customWidth="1"/>
-    <col min="4" max="4" width="3.140625" customWidth="1"/>
+    <col min="4" max="4" width="73" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -765,414 +853,511 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
+      <c r="D2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
+      <c r="D3" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
-        <v>10</v>
+      <c r="D4" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" t="s">
-        <v>13</v>
+      <c r="D5" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="C6" t="s">
-        <v>15</v>
+      <c r="D6" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>17</v>
       </c>
-      <c r="C7" t="s">
-        <v>18</v>
+      <c r="D7" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s">
-        <v>21</v>
+      <c r="D8" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" t="s">
-        <v>24</v>
+      <c r="D9" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
         <v>25</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" t="s">
-        <v>27</v>
+      <c r="D10" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" t="s">
         <v>28</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>29</v>
       </c>
-      <c r="C11" t="s">
-        <v>30</v>
+      <c r="D11" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
         <v>31</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>32</v>
       </c>
-      <c r="C12" t="s">
-        <v>33</v>
+      <c r="D12" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
         <v>34</v>
       </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
         <v>37</v>
       </c>
-      <c r="B14" t="s">
-        <v>38</v>
-      </c>
-      <c r="C14" t="s">
-        <v>38</v>
+      <c r="D14" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
         <v>39</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>40</v>
       </c>
-      <c r="C15" t="s">
-        <v>41</v>
+      <c r="D15" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
         <v>42</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>43</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
         <v>45</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>46</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" t="s">
+      <c r="B18" t="s">
         <v>48</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>49</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" t="s">
+      <c r="B19" t="s">
         <v>51</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>52</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="A20" t="s">
+      <c r="B20" t="s">
         <v>54</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>55</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
-      <c r="A21" t="s">
+      <c r="B21" t="s">
         <v>57</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>58</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
-      <c r="A22" t="s">
+      <c r="B22" t="s">
         <v>60</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>61</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
-      <c r="A23" t="s">
+      <c r="B23" t="s">
         <v>63</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>64</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" t="s">
+      <c r="B24" t="s">
         <v>66</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>67</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
-      <c r="A25" t="s">
+      <c r="B25" t="s">
         <v>69</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>70</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" t="s">
+      <c r="B26" t="s">
         <v>72</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>73</v>
       </c>
-      <c r="C26" t="s">
+      <c r="D26" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
-      <c r="A27" t="s">
+      <c r="B27" t="s">
         <v>75</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>76</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" t="s">
+      <c r="B28" t="s">
         <v>78</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>79</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
         <v>81</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>82</v>
       </c>
-      <c r="C29" t="s">
+      <c r="D29" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" t="s">
+      <c r="B30" t="s">
         <v>84</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>85</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
         <v>87</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>88</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" t="s">
+      <c r="B32" t="s">
         <v>90</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>91</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" t="s">
+      <c r="B33" t="s">
         <v>93</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>94</v>
       </c>
-      <c r="C33" t="s">
+      <c r="D33" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" t="s">
+      <c r="B34" t="s">
         <v>96</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>97</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" t="s">
+      <c r="B35" t="s">
         <v>99</v>
       </c>
-      <c r="B35" t="s">
-        <v>100</v>
-      </c>
       <c r="C35" t="s">
+        <v>99</v>
+      </c>
+      <c r="D35" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>105</v>
+      </c>
+      <c r="B36" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" t="s">
+      <c r="C36" t="s">
         <v>102</v>
       </c>
-      <c r="B36" t="s">
+      <c r="D36" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>106</v>
+      </c>
+      <c r="B37" t="s">
         <v>103</v>
       </c>
-      <c r="C36" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" t="s">
-        <v>109</v>
-      </c>
-      <c r="B37" t="s">
-        <v>105</v>
-      </c>
       <c r="C37" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" t="s">
-        <v>110</v>
-      </c>
-      <c r="B38" t="s">
-        <v>107</v>
-      </c>
-      <c r="C38" t="s">
-        <v>108</v>
+        <v>104</v>
+      </c>
+      <c r="D37" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+ line thickness widget ('choose composition method' dialog)  + new localized strings & reorganization  + configurator_eraseSettings.jsx -- delete all Glden Crop script settings from PS registry  - opacity of guidelines group changed fro 50 to 75%  - dropShadow FX replaced with white stroke FX  - WWW: SEO (metadata) optimalization  - WWW: translate with Google widget on EN site  - WWW: minor fixes
</commit_message>
<xml_diff>
--- a/translations/code/translations.xlsx
+++ b/translations/code/translations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="145">
   <si>
     <t>AvailLangs</t>
   </si>
@@ -148,24 +148,6 @@
     <t>Paski na %1%%</t>
   </si>
   <si>
-    <t>goldenDiagUp</t>
-  </si>
-  <si>
-    <t>Golden diagonal upwards</t>
-  </si>
-  <si>
-    <t>Złota przekątna w górę</t>
-  </si>
-  <si>
-    <t>goldenDiagDown</t>
-  </si>
-  <si>
-    <t>Golden diagonal downwards</t>
-  </si>
-  <si>
-    <t>Złota przekątna w dół</t>
-  </si>
-  <si>
     <t>openB4Run</t>
   </si>
   <si>
@@ -379,12 +361,6 @@
     <t>Linien auf %1%%</t>
   </si>
   <si>
-    <t>Goldene Diagonale aufwärts</t>
-  </si>
-  <si>
-    <t>Goldene Diagonale abwärts</t>
-  </si>
-  <si>
     <t>Öffne das Dokument, in dem das Script ablaufen soll.</t>
   </si>
   <si>
@@ -437,6 +413,42 @@
   </si>
   <si>
     <t>Grundregeln</t>
+  </si>
+  <si>
+    <t>goldenTriangleUp</t>
+  </si>
+  <si>
+    <t>Golden triangle upwards</t>
+  </si>
+  <si>
+    <t>Złoty trójkąt w górę</t>
+  </si>
+  <si>
+    <t>Goldene Dreieck aufwärts</t>
+  </si>
+  <si>
+    <t>goldenTriangleDown</t>
+  </si>
+  <si>
+    <t>Golden triangle downwards</t>
+  </si>
+  <si>
+    <t>Złoty trójkąt w dół</t>
+  </si>
+  <si>
+    <t>Goldene Dreieck abwärts</t>
+  </si>
+  <si>
+    <t>diagonalMethod</t>
+  </si>
+  <si>
+    <t>Diagonal method</t>
+  </si>
+  <si>
+    <t>Metoda przekątnych</t>
+  </si>
+  <si>
+    <t>Diagonale Regel</t>
   </si>
 </sst>
 </file>
@@ -830,7 +842,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
@@ -853,7 +865,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -867,7 +879,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -881,7 +893,7 @@
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -895,7 +907,7 @@
         <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -909,301 +921,301 @@
         <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>100</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>117</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D15" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="C16" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="D16" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="C17" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="D17" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C18" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="D18" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C19" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="D19" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D20" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B21" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="D21" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="D22" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C23" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="D23" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>133</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>134</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>135</v>
       </c>
       <c r="D24" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>137</v>
       </c>
       <c r="B25" t="s">
-        <v>69</v>
+        <v>138</v>
       </c>
       <c r="C25" t="s">
-        <v>70</v>
+        <v>139</v>
       </c>
       <c r="D25" t="s">
-        <v>129</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>71</v>
+        <v>141</v>
       </c>
       <c r="B26" t="s">
-        <v>72</v>
+        <v>142</v>
       </c>
       <c r="C26" t="s">
-        <v>73</v>
+        <v>143</v>
       </c>
       <c r="D26" t="s">
-        <v>130</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1217,7 +1229,7 @@
         <v>76</v>
       </c>
       <c r="D27" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1231,7 +1243,7 @@
         <v>79</v>
       </c>
       <c r="D28" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1245,7 +1257,7 @@
         <v>82</v>
       </c>
       <c r="D29" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1259,7 +1271,7 @@
         <v>85</v>
       </c>
       <c r="D30" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -1273,7 +1285,7 @@
         <v>88</v>
       </c>
       <c r="D31" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -1287,77 +1299,91 @@
         <v>91</v>
       </c>
       <c r="D32" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B33" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C33" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D33" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B34" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C34" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D34" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B35" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C35" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="D35" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" t="s">
+        <v>94</v>
+      </c>
+      <c r="B36" t="s">
+        <v>13</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36" t="s">
         <v>105</v>
-      </c>
-      <c r="B36" t="s">
-        <v>101</v>
-      </c>
-      <c r="C36" t="s">
-        <v>102</v>
-      </c>
-      <c r="D36" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>41</v>
       </c>
       <c r="B37" t="s">
-        <v>103</v>
+        <v>42</v>
       </c>
       <c r="C37" t="s">
-        <v>104</v>
+        <v>43</v>
       </c>
       <c r="D37" t="s">
-        <v>140</v>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" t="s">
+        <v>45</v>
+      </c>
+      <c r="C38" t="s">
+        <v>46</v>
+      </c>
+      <c r="D38" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- locale updated (DE)  - WWW: SEO optimization (custom <title>)
</commit_message>
<xml_diff>
--- a/translations/code/translations.xlsx
+++ b/translations/code/translations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="146">
   <si>
     <t>AvailLangs</t>
   </si>
@@ -424,9 +424,6 @@
     <t>Złoty trójkąt w górę</t>
   </si>
   <si>
-    <t>Goldene Dreieck aufwärts</t>
-  </si>
-  <si>
     <t>goldenTriangleDown</t>
   </si>
   <si>
@@ -436,9 +433,6 @@
     <t>Złoty trójkąt w dół</t>
   </si>
   <si>
-    <t>Goldene Dreieck abwärts</t>
-  </si>
-  <si>
     <t>diagonalMethod</t>
   </si>
   <si>
@@ -448,7 +442,16 @@
     <t>Metoda przekątnych</t>
   </si>
   <si>
-    <t>Diagonale Regel</t>
+    <t>Goldener Dreieck oben</t>
+  </si>
+  <si>
+    <t>Goldener Dreieck unten</t>
+  </si>
+  <si>
+    <t>Diagonale Methode</t>
+  </si>
+  <si>
+    <t>es</t>
   </si>
 </sst>
 </file>
@@ -842,19 +845,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="56.140625" customWidth="1"/>
-    <col min="3" max="3" width="53.42578125" customWidth="1"/>
-    <col min="4" max="4" width="73" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" customWidth="1"/>
+    <col min="3" max="3" width="48.7109375" customWidth="1"/>
+    <col min="4" max="4" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -867,8 +872,11 @@
       <c r="D1" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="E1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -882,7 +890,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -896,7 +904,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -910,7 +918,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -924,7 +932,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -938,7 +946,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -952,7 +960,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -966,7 +974,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -980,7 +988,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -994,7 +1002,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1008,7 +1016,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1022,7 +1030,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1036,7 +1044,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1050,284 +1058,284 @@
         <v>113</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C15" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="D15" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>50</v>
+        <v>133</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>134</v>
       </c>
       <c r="C16" t="s">
-        <v>52</v>
+        <v>135</v>
       </c>
       <c r="D16" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>136</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>137</v>
       </c>
       <c r="C17" t="s">
-        <v>55</v>
+        <v>138</v>
       </c>
       <c r="D17" t="s">
-        <v>118</v>
+        <v>143</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>139</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>140</v>
       </c>
       <c r="C18" t="s">
-        <v>58</v>
+        <v>141</v>
       </c>
       <c r="D18" t="s">
-        <v>119</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="D19" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B20" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="D20" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="C21" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="D21" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="D22" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="B23" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" t="s">
-        <v>133</v>
+        <v>59</v>
       </c>
       <c r="B24" t="s">
-        <v>134</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>135</v>
+        <v>61</v>
       </c>
       <c r="D24" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" t="s">
-        <v>137</v>
+        <v>62</v>
       </c>
       <c r="B25" t="s">
-        <v>138</v>
+        <v>63</v>
       </c>
       <c r="C25" t="s">
-        <v>139</v>
+        <v>64</v>
       </c>
       <c r="D25" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" t="s">
-        <v>141</v>
+        <v>65</v>
       </c>
       <c r="B26" t="s">
-        <v>142</v>
+        <v>66</v>
       </c>
       <c r="C26" t="s">
-        <v>143</v>
+        <v>67</v>
       </c>
       <c r="D26" t="s">
-        <v>144</v>
+        <v>122</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C28" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="D28" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B29" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C29" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="D29" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B30" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C30" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D30" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B31" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="C31" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D31" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B32" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C32" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D32" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="B33" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C33" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D33" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="B34" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C34" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="D34" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -1360,30 +1368,30 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" t="s">
-        <v>41</v>
+        <v>99</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="C37" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="D37" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="B38" t="s">
-        <v>45</v>
+        <v>97</v>
       </c>
       <c r="C38" t="s">
-        <v>46</v>
+        <v>98</v>
       </c>
       <c r="D38" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Spanish translation (thx for Cristiano007!)
</commit_message>
<xml_diff>
--- a/translations/code/translations.xlsx
+++ b/translations/code/translations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="191">
   <si>
     <t>AvailLangs</t>
   </si>
@@ -452,6 +452,141 @@
   </si>
   <si>
     <t>es</t>
+  </si>
+  <si>
+    <t>Escoja tipo de recorte</t>
+  </si>
+  <si>
+    <t>Recortar el lienzo</t>
+  </si>
+  <si>
+    <t>Hacer máscara de recorte</t>
+  </si>
+  <si>
+    <t>Fondo sobre capa</t>
+  </si>
+  <si>
+    <t>Relleno de fondo</t>
+  </si>
+  <si>
+    <t>- grilla</t>
+  </si>
+  <si>
+    <t>- re-escalar</t>
+  </si>
+  <si>
+    <t>- revelar</t>
+  </si>
+  <si>
+    <t>- recortar</t>
+  </si>
+  <si>
+    <t>Recorte Dorado por SzopeN</t>
+  </si>
+  <si>
+    <t>Máscara de recorte</t>
+  </si>
+  <si>
+    <t>Reglas de división</t>
+  </si>
+  <si>
+    <t>Cinta al %1%%</t>
+  </si>
+  <si>
+    <t>Triángulo dorado hacia arriba</t>
+  </si>
+  <si>
+    <t>Triángulo dorado hacia abajo</t>
+  </si>
+  <si>
+    <t>Método Diagonal</t>
+  </si>
+  <si>
+    <t>Abrir el documento en el cual quiere correr el script</t>
+  </si>
+  <si>
+    <t>Extensión del lienzo detectada</t>
+  </si>
+  <si>
+    <t>¿Qué hacer con el lienzo?</t>
+  </si>
+  <si>
+    <t>Extender el lienzo</t>
+  </si>
+  <si>
+    <t>Recortar sin extensón</t>
+  </si>
+  <si>
+    <t>Volver a recorte</t>
+  </si>
+  <si>
+    <t>Método de composición</t>
+  </si>
+  <si>
+    <t>Escoja guías de composición</t>
+  </si>
+  <si>
+    <t>Regla Dorada</t>
+  </si>
+  <si>
+    <t>Regla de los Tercios</t>
+  </si>
+  <si>
+    <t>Espiral Dorada abajo-izquierda</t>
+  </si>
+  <si>
+    <t>Espiral Dorada arriba-izquierda</t>
+  </si>
+  <si>
+    <t>Espiral Dorada arriba-derecha</t>
+  </si>
+  <si>
+    <t>Espiral Dorada abajo-derecha</t>
+  </si>
+  <si>
+    <t>Seleccione Todo</t>
+  </si>
+  <si>
+    <t>Deseleccione Todo</t>
+  </si>
+  <si>
+    <t>Cancelar</t>
+  </si>
+  <si>
+    <t>Todas las Espirales Doradas</t>
+  </si>
+  <si>
+    <t>Reglas Básicas</t>
+  </si>
+  <si>
+    <t>lineThickness</t>
+  </si>
+  <si>
+    <t>Line thickness</t>
+  </si>
+  <si>
+    <t>Grubość linii</t>
+  </si>
+  <si>
+    <t>Liniendicke</t>
+  </si>
+  <si>
+    <t>lineThicknessProm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Line thickness (‰ of shorter edge): </t>
+  </si>
+  <si>
+    <t>Grubość linii (‰ krótszego boku)</t>
+  </si>
+  <si>
+    <t>Liniendicke (‰ kurze Seite)</t>
+  </si>
+  <si>
+    <t>Grosor de la línea</t>
+  </si>
+  <si>
+    <t>Grosor de la línea (‰ de lado corto)</t>
   </si>
 </sst>
 </file>
@@ -486,8 +621,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -845,11 +981,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E38"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
@@ -857,6 +991,7 @@
     <col min="2" max="2" width="46.28515625" customWidth="1"/>
     <col min="3" max="3" width="48.7109375" customWidth="1"/>
     <col min="4" max="4" width="44.42578125" customWidth="1"/>
+    <col min="5" max="5" width="42.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -889,6 +1024,9 @@
       <c r="D2" t="s">
         <v>102</v>
       </c>
+      <c r="E2" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
@@ -903,6 +1041,9 @@
       <c r="D3" t="s">
         <v>102</v>
       </c>
+      <c r="E3" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
@@ -917,6 +1058,9 @@
       <c r="D4" t="s">
         <v>103</v>
       </c>
+      <c r="E4" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
@@ -931,6 +1075,9 @@
       <c r="D5" t="s">
         <v>104</v>
       </c>
+      <c r="E5" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
@@ -945,6 +1092,9 @@
       <c r="D6" t="s">
         <v>106</v>
       </c>
+      <c r="E6" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
@@ -959,6 +1109,9 @@
       <c r="D7" t="s">
         <v>107</v>
       </c>
+      <c r="E7" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
@@ -973,6 +1126,9 @@
       <c r="D8" t="s">
         <v>108</v>
       </c>
+      <c r="E8" s="1" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
@@ -987,6 +1143,9 @@
       <c r="D9" t="s">
         <v>109</v>
       </c>
+      <c r="E9" s="1" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
@@ -1001,6 +1160,9 @@
       <c r="D10" t="s">
         <v>110</v>
       </c>
+      <c r="E10" s="1" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
@@ -1015,6 +1177,9 @@
       <c r="D11" t="s">
         <v>111</v>
       </c>
+      <c r="E11" s="1" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
@@ -1029,6 +1194,9 @@
       <c r="D12" t="s">
         <v>34</v>
       </c>
+      <c r="E12" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
@@ -1043,6 +1211,9 @@
       <c r="D13" t="s">
         <v>112</v>
       </c>
+      <c r="E13" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
@@ -1057,6 +1228,9 @@
       <c r="D14" t="s">
         <v>113</v>
       </c>
+      <c r="E14" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
@@ -1071,6 +1245,9 @@
       <c r="D15" t="s">
         <v>114</v>
       </c>
+      <c r="E15" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
@@ -1085,8 +1262,11 @@
       <c r="D16" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -1099,8 +1279,11 @@
       <c r="D17" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>139</v>
       </c>
@@ -1113,8 +1296,11 @@
       <c r="D18" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -1127,8 +1313,11 @@
       <c r="D19" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -1141,8 +1330,11 @@
       <c r="D20" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -1155,8 +1347,11 @@
       <c r="D21" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -1169,8 +1364,11 @@
       <c r="D22" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -1183,8 +1381,11 @@
       <c r="D23" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="E23" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -1197,8 +1398,11 @@
       <c r="D24" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="25" spans="1:4">
+      <c r="E24" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -1211,8 +1415,11 @@
       <c r="D25" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="E25" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -1225,8 +1432,11 @@
       <c r="D26" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="E26" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>68</v>
       </c>
@@ -1239,8 +1449,11 @@
       <c r="D27" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="E27" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>71</v>
       </c>
@@ -1253,8 +1466,11 @@
       <c r="D28" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="29" spans="1:4">
+      <c r="E28" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>74</v>
       </c>
@@ -1267,8 +1483,11 @@
       <c r="D29" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>77</v>
       </c>
@@ -1281,8 +1500,11 @@
       <c r="D30" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="31" spans="1:4">
+      <c r="E30" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>80</v>
       </c>
@@ -1295,8 +1517,11 @@
       <c r="D31" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="32" spans="1:4">
+      <c r="E31" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>83</v>
       </c>
@@ -1309,8 +1534,11 @@
       <c r="D32" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="33" spans="1:4">
+      <c r="E32" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>86</v>
       </c>
@@ -1323,8 +1551,11 @@
       <c r="D33" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="34" spans="1:4">
+      <c r="E33" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>89</v>
       </c>
@@ -1337,8 +1568,11 @@
       <c r="D34" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="35" spans="1:4">
+      <c r="E34" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>92</v>
       </c>
@@ -1351,8 +1585,11 @@
       <c r="D35" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="36" spans="1:4">
+      <c r="E35" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>94</v>
       </c>
@@ -1365,8 +1602,11 @@
       <c r="D36" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="37" spans="1:4">
+      <c r="E36" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>99</v>
       </c>
@@ -1379,8 +1619,11 @@
       <c r="D37" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="38" spans="1:4">
+      <c r="E37" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>100</v>
       </c>
@@ -1392,6 +1635,43 @@
       </c>
       <c r="D38" t="s">
         <v>132</v>
+      </c>
+      <c r="E38" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>181</v>
+      </c>
+      <c r="B39" t="s">
+        <v>182</v>
+      </c>
+      <c r="C39" t="s">
+        <v>183</v>
+      </c>
+      <c r="D39" t="s">
+        <v>184</v>
+      </c>
+      <c r="E39" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>185</v>
+      </c>
+      <c r="B40" t="s">
+        <v>186</v>
+      </c>
+      <c r="C40" t="s">
+        <v>187</v>
+      </c>
+      <c r="D40" t="s">
+        <v>188</v>
+      </c>
+      <c r="E40" t="s">
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
+ Russian translation [Vlad Kovnerov] - pre rel -
</commit_message>
<xml_diff>
--- a/translations/code/translations.xlsx
+++ b/translations/code/translations.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="189"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="230">
   <si>
     <t>AvailLangs</t>
   </si>
@@ -587,6 +587,123 @@
   </si>
   <si>
     <t>Grosor de la línea (‰ de lado corto)</t>
+  </si>
+  <si>
+    <t>ru</t>
+  </si>
+  <si>
+    <t>Вид кадрирования</t>
+  </si>
+  <si>
+    <t>Выберите вид кадрирования</t>
+  </si>
+  <si>
+    <t>Обрезать холст</t>
+  </si>
+  <si>
+    <t>Создать маску</t>
+  </si>
+  <si>
+    <t>Фоновый слой</t>
+  </si>
+  <si>
+    <t>Фоновая заливка</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - сетка</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - размер</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - показ</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - обрезка</t>
+  </si>
+  <si>
+    <t>Golden Crop от SzopeN</t>
+  </si>
+  <si>
+    <t>Маска кадрирвания</t>
+  </si>
+  <si>
+    <t>Правила разделения</t>
+  </si>
+  <si>
+    <t>Линии на %1%%</t>
+  </si>
+  <si>
+    <t>Золотой треугольник вверх</t>
+  </si>
+  <si>
+    <t>Золотой треугольник вниз</t>
+  </si>
+  <si>
+    <t>Метод диагоналей</t>
+  </si>
+  <si>
+    <t>Откройте файл, в котором вы хотели бы запустить скрипт.</t>
+  </si>
+  <si>
+    <t>Обнаружено увеличение холста</t>
+  </si>
+  <si>
+    <t>Что следует предпринять?</t>
+  </si>
+  <si>
+    <t>Увеличить размеры</t>
+  </si>
+  <si>
+    <t>Обрезать без увеличения</t>
+  </si>
+  <si>
+    <t>Вернуться к кадрированию</t>
+  </si>
+  <si>
+    <t>Метод построения композиции</t>
+  </si>
+  <si>
+    <t>Выберите тип направляющих линий</t>
+  </si>
+  <si>
+    <t>Золотое сечение</t>
+  </si>
+  <si>
+    <t>Правило третей</t>
+  </si>
+  <si>
+    <t>Золотая спираль внизу-слева</t>
+  </si>
+  <si>
+    <t>Золотая спираль вверху-слева</t>
+  </si>
+  <si>
+    <t>Золотая спираль вверху-справа</t>
+  </si>
+  <si>
+    <t>Золотая спираль внизу-справа</t>
+  </si>
+  <si>
+    <t>Выбрать все</t>
+  </si>
+  <si>
+    <t>Убрать все</t>
+  </si>
+  <si>
+    <t>Отмена</t>
+  </si>
+  <si>
+    <t>Все золотые спирали</t>
+  </si>
+  <si>
+    <t>Основные правила</t>
+  </si>
+  <si>
+    <t>Толщина линий</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Толщина линий (‰ меньшей стороны): </t>
   </si>
 </sst>
 </file>
@@ -981,9 +1098,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
@@ -992,9 +1111,10 @@
     <col min="3" max="3" width="48.7109375" customWidth="1"/>
     <col min="4" max="4" width="44.42578125" customWidth="1"/>
     <col min="5" max="5" width="42.42578125" customWidth="1"/>
+    <col min="6" max="6" width="53.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1010,8 +1130,11 @@
       <c r="E1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1027,8 +1150,11 @@
       <c r="E2" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1044,8 +1170,11 @@
       <c r="E3" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1061,8 +1190,11 @@
       <c r="E4" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1078,8 +1210,11 @@
       <c r="E5" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1095,8 +1230,11 @@
       <c r="E6" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1112,8 +1250,11 @@
       <c r="E7" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1129,8 +1270,11 @@
       <c r="E8" s="1" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1146,8 +1290,11 @@
       <c r="E9" s="1" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1163,8 +1310,11 @@
       <c r="E10" s="1" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1180,8 +1330,11 @@
       <c r="E11" s="1" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1197,8 +1350,11 @@
       <c r="E12" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1214,8 +1370,11 @@
       <c r="E13" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
+      <c r="F13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1231,8 +1390,11 @@
       <c r="E14" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="15" spans="1:5">
+      <c r="F14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -1248,8 +1410,11 @@
       <c r="E15" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="16" spans="1:5">
+      <c r="F15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" t="s">
         <v>133</v>
       </c>
@@ -1265,8 +1430,11 @@
       <c r="E16" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="17" spans="1:5">
+      <c r="F16" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -1282,8 +1450,11 @@
       <c r="E17" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
+      <c r="F17" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>139</v>
       </c>
@@ -1299,8 +1470,11 @@
       <c r="E18" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -1316,8 +1490,11 @@
       <c r="E19" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="20" spans="1:5">
+      <c r="F19" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -1333,8 +1510,11 @@
       <c r="E20" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
+      <c r="F20" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -1350,8 +1530,11 @@
       <c r="E21" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="F21" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -1367,8 +1550,11 @@
       <c r="E22" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="23" spans="1:5">
+      <c r="F22" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -1384,8 +1570,11 @@
       <c r="E23" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="24" spans="1:5">
+      <c r="F23" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -1401,8 +1590,11 @@
       <c r="E24" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -1418,8 +1610,11 @@
       <c r="E25" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="26" spans="1:5">
+      <c r="F25" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -1435,8 +1630,11 @@
       <c r="E26" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="F26" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="s">
         <v>68</v>
       </c>
@@ -1452,8 +1650,11 @@
       <c r="E27" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="28" spans="1:5">
+      <c r="F27" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="s">
         <v>71</v>
       </c>
@@ -1469,8 +1670,11 @@
       <c r="E28" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="s">
         <v>74</v>
       </c>
@@ -1486,8 +1690,11 @@
       <c r="E29" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="30" spans="1:5">
+      <c r="F29" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="s">
         <v>77</v>
       </c>
@@ -1503,8 +1710,11 @@
       <c r="E30" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="31" spans="1:5">
+      <c r="F30" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" t="s">
         <v>80</v>
       </c>
@@ -1520,8 +1730,11 @@
       <c r="E31" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="32" spans="1:5">
+      <c r="F31" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32" t="s">
         <v>83</v>
       </c>
@@ -1537,8 +1750,11 @@
       <c r="E32" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="33" spans="1:5">
+      <c r="F32" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33" t="s">
         <v>86</v>
       </c>
@@ -1554,8 +1770,11 @@
       <c r="E33" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="34" spans="1:5">
+      <c r="F33" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" t="s">
         <v>89</v>
       </c>
@@ -1571,8 +1790,11 @@
       <c r="E34" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="35" spans="1:5">
+      <c r="F34" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35" t="s">
         <v>92</v>
       </c>
@@ -1588,8 +1810,11 @@
       <c r="E35" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="36" spans="1:5">
+      <c r="F35" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36" t="s">
         <v>94</v>
       </c>
@@ -1605,8 +1830,11 @@
       <c r="E36" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="37" spans="1:5">
+      <c r="F36" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" t="s">
         <v>99</v>
       </c>
@@ -1622,8 +1850,11 @@
       <c r="E37" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="38" spans="1:5">
+      <c r="F37" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38" t="s">
         <v>100</v>
       </c>
@@ -1639,8 +1870,11 @@
       <c r="E38" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="39" spans="1:5">
+      <c r="F38" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39" t="s">
         <v>181</v>
       </c>
@@ -1656,8 +1890,11 @@
       <c r="E39" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="40" spans="1:5">
+      <c r="F39" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" t="s">
         <v>185</v>
       </c>
@@ -1672,6 +1909,9 @@
       </c>
       <c r="E40" t="s">
         <v>190</v>
+      </c>
+      <c r="F40" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Locale goldenSpiral added for all languages [en,pl,de,es,ru]
</commit_message>
<xml_diff>
--- a/translations/code/translations.xlsx
+++ b/translations/code/translations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="236">
   <si>
     <t>AvailLangs</t>
   </si>
@@ -704,6 +704,24 @@
   </si>
   <si>
     <t xml:space="preserve">Толщина линий (‰ меньшей стороны): </t>
+  </si>
+  <si>
+    <t>goldenSpiral</t>
+  </si>
+  <si>
+    <t>Golden Spiral</t>
+  </si>
+  <si>
+    <t>Złota spirala</t>
+  </si>
+  <si>
+    <t>Goldene Spirale</t>
+  </si>
+  <si>
+    <t>Espiral Dorada</t>
+  </si>
+  <si>
+    <t>Золотая спираль</t>
   </si>
 </sst>
 </file>
@@ -1098,20 +1116,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="46.28515625" customWidth="1"/>
-    <col min="3" max="3" width="48.7109375" customWidth="1"/>
-    <col min="4" max="4" width="44.42578125" customWidth="1"/>
-    <col min="5" max="5" width="42.42578125" customWidth="1"/>
-    <col min="6" max="6" width="53.42578125" customWidth="1"/>
+    <col min="2" max="2" width="48" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="50.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="52.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1756,161 +1774,181 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>86</v>
+        <v>230</v>
       </c>
       <c r="B33" t="s">
-        <v>87</v>
+        <v>231</v>
       </c>
       <c r="C33" t="s">
-        <v>88</v>
+        <v>232</v>
       </c>
       <c r="D33" t="s">
-        <v>129</v>
+        <v>233</v>
       </c>
       <c r="E33" t="s">
-        <v>176</v>
+        <v>234</v>
       </c>
       <c r="F33" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
     </row>
     <row r="34" spans="1:6">
       <c r="A34" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B34" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C34" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D34" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E34" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="F34" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B35" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C35" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D35" t="s">
-        <v>93</v>
+        <v>130</v>
       </c>
       <c r="E35" t="s">
-        <v>93</v>
+        <v>177</v>
       </c>
       <c r="F35" t="s">
-        <v>93</v>
+        <v>224</v>
       </c>
     </row>
     <row r="36" spans="1:6">
       <c r="A36" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B36" t="s">
-        <v>13</v>
+        <v>93</v>
       </c>
       <c r="C36" t="s">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="D36" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="E36" t="s">
-        <v>178</v>
+        <v>93</v>
       </c>
       <c r="F36" t="s">
-        <v>225</v>
+        <v>93</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="A37" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B37" t="s">
-        <v>95</v>
+        <v>13</v>
       </c>
       <c r="C37" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="D37" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="E37" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="F37" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B38" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C38" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E38" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F38" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="39" spans="1:6">
       <c r="A39" t="s">
-        <v>181</v>
+        <v>100</v>
       </c>
       <c r="B39" t="s">
-        <v>182</v>
+        <v>97</v>
       </c>
       <c r="C39" t="s">
-        <v>183</v>
+        <v>98</v>
       </c>
       <c r="D39" t="s">
-        <v>184</v>
+        <v>132</v>
       </c>
       <c r="E39" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="F39" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="40" spans="1:6">
       <c r="A40" t="s">
+        <v>181</v>
+      </c>
+      <c r="B40" t="s">
+        <v>182</v>
+      </c>
+      <c r="C40" t="s">
+        <v>183</v>
+      </c>
+      <c r="D40" t="s">
+        <v>184</v>
+      </c>
+      <c r="E40" t="s">
+        <v>189</v>
+      </c>
+      <c r="F40" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
         <v>185</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>186</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>187</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>188</v>
       </c>
-      <c r="E40" t="s">
+      <c r="E41" t="s">
         <v>190</v>
       </c>
-      <c r="F40" t="s">
+      <c r="F41" t="s">
         <v>229</v>
       </c>
     </row>

</xml_diff>

<commit_message>
0.92a -- added Italian translation (thx Mantra) WWW minor fixes (credits, no-cache)
</commit_message>
<xml_diff>
--- a/translations/code/translations.xlsx
+++ b/translations/code/translations.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="275">
   <si>
     <t>AvailLangs</t>
   </si>
@@ -469,18 +469,6 @@
     <t>Relleno de fondo</t>
   </si>
   <si>
-    <t>- grilla</t>
-  </si>
-  <si>
-    <t>- re-escalar</t>
-  </si>
-  <si>
-    <t>- revelar</t>
-  </si>
-  <si>
-    <t>- recortar</t>
-  </si>
-  <si>
     <t>Recorte Dorado por SzopeN</t>
   </si>
   <si>
@@ -722,6 +710,135 @@
   </si>
   <si>
     <t>Золотая спираль</t>
+  </si>
+  <si>
+    <t>it</t>
+  </si>
+  <si>
+    <t>Scegli stile taglieria</t>
+  </si>
+  <si>
+    <t>Taglieria (Semplice taglieria)</t>
+  </si>
+  <si>
+    <t>Crea maschera taglieria</t>
+  </si>
+  <si>
+    <t>Sfondo del livello</t>
+  </si>
+  <si>
+    <t>Riempimento sfondo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - griglia</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - cambia dimensioni</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - rivela</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - taglia</t>
+  </si>
+  <si>
+    <t>Taglieria d'oro di SzopeN</t>
+  </si>
+  <si>
+    <t>Mascheria taglieria</t>
+  </si>
+  <si>
+    <t>Regole della divisione</t>
+  </si>
+  <si>
+    <t>Guida a %1%%</t>
+  </si>
+  <si>
+    <t>Triangolo d'oro all'insù</t>
+  </si>
+  <si>
+    <t>Triangolo d'oro all'ingiù</t>
+  </si>
+  <si>
+    <t>Metodo Diagonale</t>
+  </si>
+  <si>
+    <t>Apri il documento nel quale vuoi applicare lo script.</t>
+  </si>
+  <si>
+    <t>Estensione quadro  trovato.</t>
+  </si>
+  <si>
+    <t>Cosa fare con il quatro?</t>
+  </si>
+  <si>
+    <t>Esteso quadro</t>
+  </si>
+  <si>
+    <t>taglia senza estensione</t>
+  </si>
+  <si>
+    <t>Torna alla taglieria</t>
+  </si>
+  <si>
+    <t>Metodo di composizione</t>
+  </si>
+  <si>
+    <t>Sciegli guide di composizione</t>
+  </si>
+  <si>
+    <t>Regola d'oro</t>
+  </si>
+  <si>
+    <t>Regola dei terzi</t>
+  </si>
+  <si>
+    <t>Spirale d'oro in basso a sinistra</t>
+  </si>
+  <si>
+    <t>Spirale d'oro in alto a sinistra</t>
+  </si>
+  <si>
+    <t>Spirale d'oro in alto a destra</t>
+  </si>
+  <si>
+    <t>Spirale d'oro in basso a destra</t>
+  </si>
+  <si>
+    <t>Spirale d'oro</t>
+  </si>
+  <si>
+    <t>Seleziona Tutto</t>
+  </si>
+  <si>
+    <t>Deselezionare Tutto</t>
+  </si>
+  <si>
+    <t>cancellare</t>
+  </si>
+  <si>
+    <t>Tutte le spirali d'oro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regole fondamentali </t>
+  </si>
+  <si>
+    <t>Grossezza guida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grossezza guida (‰ di taglio più corto): </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - grilla</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - re-escalar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - revelar</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - recortar</t>
   </si>
 </sst>
 </file>
@@ -756,9 +873,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1116,11 +1232,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
@@ -1130,9 +1244,10 @@
     <col min="4" max="4" width="46.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="44.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="52.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1149,10 +1264,13 @@
         <v>145</v>
       </c>
       <c r="F1" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+        <v>187</v>
+      </c>
+      <c r="G1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1169,10 +1287,13 @@
         <v>146</v>
       </c>
       <c r="F2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>188</v>
+      </c>
+      <c r="G2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1189,10 +1310,13 @@
         <v>146</v>
       </c>
       <c r="F3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>189</v>
+      </c>
+      <c r="G3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1209,10 +1333,13 @@
         <v>147</v>
       </c>
       <c r="F4" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>190</v>
+      </c>
+      <c r="G4" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1229,10 +1356,13 @@
         <v>148</v>
       </c>
       <c r="F5" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>191</v>
+      </c>
+      <c r="G5" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1249,10 +1379,13 @@
         <v>149</v>
       </c>
       <c r="F6" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>192</v>
+      </c>
+      <c r="G6" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -1269,10 +1402,13 @@
         <v>150</v>
       </c>
       <c r="F7" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>193</v>
+      </c>
+      <c r="G7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1285,14 +1421,17 @@
       <c r="D8" t="s">
         <v>108</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>151</v>
+      <c r="E8" t="s">
+        <v>271</v>
       </c>
       <c r="F8" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>194</v>
+      </c>
+      <c r="G8" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1305,14 +1444,17 @@
       <c r="D9" t="s">
         <v>109</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>152</v>
+      <c r="E9" t="s">
+        <v>272</v>
       </c>
       <c r="F9" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>195</v>
+      </c>
+      <c r="G9" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -1325,14 +1467,17 @@
       <c r="D10" t="s">
         <v>110</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>153</v>
+      <c r="E10" t="s">
+        <v>273</v>
       </c>
       <c r="F10" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>196</v>
+      </c>
+      <c r="G10" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1345,14 +1490,17 @@
       <c r="D11" t="s">
         <v>111</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>154</v>
+      <c r="E11" t="s">
+        <v>274</v>
       </c>
       <c r="F11" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>197</v>
+      </c>
+      <c r="G11" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1366,13 +1514,16 @@
         <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F12" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>198</v>
+      </c>
+      <c r="G12" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1386,13 +1537,16 @@
         <v>112</v>
       </c>
       <c r="E13" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="F13" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>199</v>
+      </c>
+      <c r="G13" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -1406,13 +1560,16 @@
         <v>113</v>
       </c>
       <c r="E14" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F14" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>200</v>
+      </c>
+      <c r="G14" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
       <c r="A15" t="s">
         <v>41</v>
       </c>
@@ -1426,13 +1583,16 @@
         <v>114</v>
       </c>
       <c r="E15" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F15" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>201</v>
+      </c>
+      <c r="G15" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
       <c r="A16" t="s">
         <v>133</v>
       </c>
@@ -1446,13 +1606,16 @@
         <v>142</v>
       </c>
       <c r="E16" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F16" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>202</v>
+      </c>
+      <c r="G16" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>136</v>
       </c>
@@ -1466,13 +1629,16 @@
         <v>143</v>
       </c>
       <c r="E17" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="F17" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>203</v>
+      </c>
+      <c r="G17" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>139</v>
       </c>
@@ -1486,13 +1652,16 @@
         <v>144</v>
       </c>
       <c r="E18" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="F18" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+        <v>204</v>
+      </c>
+      <c r="G18" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>44</v>
       </c>
@@ -1506,13 +1675,16 @@
         <v>115</v>
       </c>
       <c r="E19" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F19" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>205</v>
+      </c>
+      <c r="G19" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>47</v>
       </c>
@@ -1526,13 +1698,16 @@
         <v>116</v>
       </c>
       <c r="E20" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="F20" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>206</v>
+      </c>
+      <c r="G20" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -1546,13 +1721,16 @@
         <v>117</v>
       </c>
       <c r="E21" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="F21" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>207</v>
+      </c>
+      <c r="G21" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -1566,13 +1744,16 @@
         <v>118</v>
       </c>
       <c r="E22" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="F22" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>208</v>
+      </c>
+      <c r="G22" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>56</v>
       </c>
@@ -1586,13 +1767,16 @@
         <v>119</v>
       </c>
       <c r="E23" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="F23" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
+        <v>209</v>
+      </c>
+      <c r="G23" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -1606,13 +1790,16 @@
         <v>120</v>
       </c>
       <c r="E24" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="F24" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>210</v>
+      </c>
+      <c r="G24" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>62</v>
       </c>
@@ -1626,13 +1813,16 @@
         <v>121</v>
       </c>
       <c r="E25" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="F25" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>211</v>
+      </c>
+      <c r="G25" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>65</v>
       </c>
@@ -1646,13 +1836,16 @@
         <v>122</v>
       </c>
       <c r="E26" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="F26" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>212</v>
+      </c>
+      <c r="G26" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>68</v>
       </c>
@@ -1666,13 +1859,16 @@
         <v>123</v>
       </c>
       <c r="E27" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="F27" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>213</v>
+      </c>
+      <c r="G27" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>71</v>
       </c>
@@ -1686,13 +1882,16 @@
         <v>124</v>
       </c>
       <c r="E28" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="F28" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6">
+        <v>214</v>
+      </c>
+      <c r="G28" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>74</v>
       </c>
@@ -1706,13 +1905,16 @@
         <v>125</v>
       </c>
       <c r="E29" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="F29" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>215</v>
+      </c>
+      <c r="G29" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>77</v>
       </c>
@@ -1726,13 +1928,16 @@
         <v>126</v>
       </c>
       <c r="E30" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="F30" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>216</v>
+      </c>
+      <c r="G30" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>80</v>
       </c>
@@ -1746,13 +1951,16 @@
         <v>127</v>
       </c>
       <c r="E31" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="F31" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>217</v>
+      </c>
+      <c r="G31" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>83</v>
       </c>
@@ -1766,33 +1974,39 @@
         <v>128</v>
       </c>
       <c r="E32" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="F32" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>218</v>
+      </c>
+      <c r="G32" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
+        <v>226</v>
+      </c>
+      <c r="B33" t="s">
+        <v>227</v>
+      </c>
+      <c r="C33" t="s">
+        <v>228</v>
+      </c>
+      <c r="D33" t="s">
+        <v>229</v>
+      </c>
+      <c r="E33" t="s">
         <v>230</v>
       </c>
-      <c r="B33" t="s">
+      <c r="F33" t="s">
         <v>231</v>
       </c>
-      <c r="C33" t="s">
-        <v>232</v>
-      </c>
-      <c r="D33" t="s">
-        <v>233</v>
-      </c>
-      <c r="E33" t="s">
-        <v>234</v>
-      </c>
-      <c r="F33" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>86</v>
       </c>
@@ -1806,13 +2020,16 @@
         <v>129</v>
       </c>
       <c r="E34" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F34" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>219</v>
+      </c>
+      <c r="G34" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>89</v>
       </c>
@@ -1826,13 +2043,16 @@
         <v>130</v>
       </c>
       <c r="E35" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F35" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6">
+        <v>220</v>
+      </c>
+      <c r="G35" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>92</v>
       </c>
@@ -1851,8 +2071,11 @@
       <c r="F36" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G36" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>94</v>
       </c>
@@ -1866,13 +2089,16 @@
         <v>105</v>
       </c>
       <c r="E37" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F37" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>221</v>
+      </c>
+      <c r="G37" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>99</v>
       </c>
@@ -1886,13 +2112,16 @@
         <v>131</v>
       </c>
       <c r="E38" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="F38" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6">
+        <v>222</v>
+      </c>
+      <c r="G38" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>100</v>
       </c>
@@ -1906,50 +2135,59 @@
         <v>132</v>
       </c>
       <c r="E39" t="s">
+        <v>176</v>
+      </c>
+      <c r="F39" t="s">
+        <v>223</v>
+      </c>
+      <c r="G39" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" t="s">
+        <v>177</v>
+      </c>
+      <c r="B40" t="s">
+        <v>178</v>
+      </c>
+      <c r="C40" t="s">
+        <v>179</v>
+      </c>
+      <c r="D40" t="s">
         <v>180</v>
       </c>
-      <c r="F39" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" t="s">
+      <c r="E40" t="s">
+        <v>185</v>
+      </c>
+      <c r="F40" t="s">
+        <v>224</v>
+      </c>
+      <c r="G40" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
         <v>181</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B41" t="s">
         <v>182</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>183</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>184</v>
       </c>
-      <c r="E40" t="s">
-        <v>189</v>
-      </c>
-      <c r="F40" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" t="s">
-        <v>185</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="E41" t="s">
         <v>186</v>
       </c>
-      <c r="C41" t="s">
-        <v>187</v>
-      </c>
-      <c r="D41" t="s">
-        <v>188</v>
-      </c>
-      <c r="E41" t="s">
-        <v>190</v>
-      </c>
       <c r="F41" t="s">
-        <v>229</v>
+        <v>225</v>
+      </c>
+      <c r="G41" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>

</xml_diff>